<commit_message>
paralle ex added, data provider with excel added
</commit_message>
<xml_diff>
--- a/studentDetails.xlsx
+++ b/studentDetails.xlsx
@@ -12,15 +12,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
   <si>
     <t/>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Age</t>
   </si>
   <si>
     <t>Amal</t>
@@ -74,7 +68,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -84,31 +78,23 @@
       <c r="A1" t="s" s="0">
         <v>1</v>
       </c>
-      <c r="B1" t="s" s="0">
-        <v>2</v>
+      <c r="B1" t="n" s="0">
+        <v>25.0</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" t="n" s="0">
-        <v>25.0</v>
+        <v>30.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" t="n" s="0">
-        <v>30.0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s" s="0">
-        <v>5</v>
-      </c>
-      <c r="B4" t="n" s="0">
         <v>28.0</v>
       </c>
     </row>

</xml_diff>